<commit_message>
changed colours of table
</commit_message>
<xml_diff>
--- a/assets/elements.xlsx
+++ b/assets/elements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="371">
   <si>
     <t>symbol</t>
   </si>
@@ -802,12 +802,6 @@
   </si>
   <si>
     <t>From the Greek words "nitron genes" meaning "nitre" and "forming" and the Latin word "nitrum" (nitre is a common name for potassium nitrate, KNO#)</t>
-  </si>
-  <si>
-    <t>More history of the names can be found on:</t>
-  </si>
-  <si>
-    <t>https://www.webelements.com</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -1410,12 +1404,6 @@
     <t>Named after the State and University of "California", USA</t>
   </si>
   <si>
-    <t>https://www.ca.gov</t>
-  </si>
-  <si>
-    <t>https://www.universityofcalifornia.edu</t>
-  </si>
-  <si>
     <t>Named after "Albert Einstein"</t>
   </si>
   <si>
@@ -1426,9 +1414,6 @@
   </si>
   <si>
     <t>Named after Alfred Bernhard "Nobel", Swedish chemist who discovered dynamite, and founder of the Nobel Prizes</t>
-  </si>
-  <si>
-    <t>https://www.nobelprize.org</t>
   </si>
 </sst>
 </file>
@@ -1808,10 +1793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C100" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +1984,7 @@
         <v>246</v>
       </c>
       <c r="F9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2004,7 @@
         <v>246</v>
       </c>
       <c r="F10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,7 +2025,7 @@
         <v>Noble Gas</v>
       </c>
       <c r="F11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2060,7 +2045,7 @@
         <v>245</v>
       </c>
       <c r="F12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2080,7 +2065,7 @@
         <v>243</v>
       </c>
       <c r="F13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2100,7 +2085,7 @@
         <v>248</v>
       </c>
       <c r="F14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2120,7 +2105,7 @@
         <v>247</v>
       </c>
       <c r="F15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2140,7 +2125,7 @@
         <v>246</v>
       </c>
       <c r="F16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2160,7 +2145,7 @@
         <v>246</v>
       </c>
       <c r="F17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2180,7 +2165,7 @@
         <v>246</v>
       </c>
       <c r="F18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2201,7 +2186,7 @@
         <v>Noble Gas</v>
       </c>
       <c r="F19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2221,7 +2206,7 @@
         <v>245</v>
       </c>
       <c r="F20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2241,7 +2226,7 @@
         <v>243</v>
       </c>
       <c r="F21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2261,7 +2246,7 @@
         <v>249</v>
       </c>
       <c r="F22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2281,7 +2266,7 @@
         <v>249</v>
       </c>
       <c r="F23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2301,7 +2286,7 @@
         <v>249</v>
       </c>
       <c r="F24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2321,7 +2306,7 @@
         <v>249</v>
       </c>
       <c r="F25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2341,7 +2326,7 @@
         <v>249</v>
       </c>
       <c r="F26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2361,7 +2346,7 @@
         <v>249</v>
       </c>
       <c r="F27" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2381,7 +2366,7 @@
         <v>249</v>
       </c>
       <c r="F28" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2401,7 +2386,7 @@
         <v>249</v>
       </c>
       <c r="F29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2421,7 +2406,7 @@
         <v>249</v>
       </c>
       <c r="F30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2441,7 +2426,7 @@
         <v>249</v>
       </c>
       <c r="F31" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2461,7 +2446,7 @@
         <v>248</v>
       </c>
       <c r="F32" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,7 +2466,7 @@
         <v>247</v>
       </c>
       <c r="F33" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2501,7 +2486,7 @@
         <v>247</v>
       </c>
       <c r="F34" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2521,7 +2506,7 @@
         <v>246</v>
       </c>
       <c r="F35" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2541,7 +2526,7 @@
         <v>246</v>
       </c>
       <c r="F36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2561,7 +2546,7 @@
         <v>240</v>
       </c>
       <c r="F37" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2581,7 +2566,7 @@
         <v>245</v>
       </c>
       <c r="F38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2601,7 +2586,7 @@
         <v>243</v>
       </c>
       <c r="F39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2621,7 +2606,7 @@
         <v>249</v>
       </c>
       <c r="F40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2641,7 +2626,7 @@
         <v>249</v>
       </c>
       <c r="F41" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2661,7 +2646,7 @@
         <v>249</v>
       </c>
       <c r="F42" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2681,7 +2666,7 @@
         <v>249</v>
       </c>
       <c r="F43" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2701,7 +2686,7 @@
         <v>249</v>
       </c>
       <c r="F44" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2721,7 +2706,7 @@
         <v>249</v>
       </c>
       <c r="F45" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2741,7 +2726,7 @@
         <v>249</v>
       </c>
       <c r="F46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2761,7 +2746,7 @@
         <v>249</v>
       </c>
       <c r="F47" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2781,7 +2766,7 @@
         <v>249</v>
       </c>
       <c r="F48" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2801,7 +2786,7 @@
         <v>249</v>
       </c>
       <c r="F49" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2821,7 +2806,7 @@
         <v>248</v>
       </c>
       <c r="F50" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,7 +2826,7 @@
         <v>248</v>
       </c>
       <c r="F51" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2861,7 +2846,7 @@
         <v>247</v>
       </c>
       <c r="F52" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2881,7 +2866,7 @@
         <v>247</v>
       </c>
       <c r="F53" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2901,7 +2886,7 @@
         <v>246</v>
       </c>
       <c r="F54" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,7 +2907,7 @@
         <v>Noble Gas</v>
       </c>
       <c r="F55" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2942,7 +2927,7 @@
         <v>245</v>
       </c>
       <c r="F56" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2962,7 +2947,7 @@
         <v>243</v>
       </c>
       <c r="F57" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2982,7 +2967,7 @@
         <v>249</v>
       </c>
       <c r="F58" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3002,7 +2987,7 @@
         <v>249</v>
       </c>
       <c r="F59" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,7 +3007,7 @@
         <v>249</v>
       </c>
       <c r="F60" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,7 +3027,7 @@
         <v>249</v>
       </c>
       <c r="F61" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -3062,7 +3047,7 @@
         <v>249</v>
       </c>
       <c r="F62" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,7 +3067,7 @@
         <v>249</v>
       </c>
       <c r="F63" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3102,7 +3087,7 @@
         <v>249</v>
       </c>
       <c r="F64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -3122,7 +3107,7 @@
         <v>249</v>
       </c>
       <c r="F65" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -3142,7 +3127,7 @@
         <v>249</v>
       </c>
       <c r="F66" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,7 +3147,7 @@
         <v>248</v>
       </c>
       <c r="F67" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -3182,7 +3167,7 @@
         <v>248</v>
       </c>
       <c r="F68" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3202,7 +3187,7 @@
         <v>248</v>
       </c>
       <c r="F69" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3222,7 +3207,7 @@
         <v>248</v>
       </c>
       <c r="F70" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,7 +3227,7 @@
         <v>247</v>
       </c>
       <c r="F71" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3263,7 +3248,7 @@
         <v>Noble Gas</v>
       </c>
       <c r="F72" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -3283,7 +3268,7 @@
         <v>245</v>
       </c>
       <c r="F73" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3303,7 +3288,7 @@
         <v>243</v>
       </c>
       <c r="F74" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3323,7 +3308,7 @@
         <v>249</v>
       </c>
       <c r="F75" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3343,7 +3328,7 @@
         <v>249</v>
       </c>
       <c r="F76" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3363,7 +3348,7 @@
         <v>249</v>
       </c>
       <c r="F77" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3383,7 +3368,7 @@
         <v>249</v>
       </c>
       <c r="F78" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -3403,7 +3388,7 @@
         <v>249</v>
       </c>
       <c r="F79" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3423,7 +3408,7 @@
         <v>250</v>
       </c>
       <c r="F80" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3443,7 +3428,7 @@
         <v>250</v>
       </c>
       <c r="F81" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -3463,7 +3448,7 @@
         <v>250</v>
       </c>
       <c r="F82" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3483,7 +3468,7 @@
         <v>250</v>
       </c>
       <c r="F83" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3503,7 +3488,7 @@
         <v>250</v>
       </c>
       <c r="F84" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -3523,7 +3508,7 @@
         <v>250</v>
       </c>
       <c r="F85" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3543,7 +3528,7 @@
         <v>251</v>
       </c>
       <c r="F86" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3563,7 +3548,7 @@
         <v>252</v>
       </c>
       <c r="F87" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3583,7 +3568,7 @@
         <v>253</v>
       </c>
       <c r="F88" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3603,7 +3588,7 @@
         <v>240</v>
       </c>
       <c r="F89" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3623,7 +3608,7 @@
         <v>241</v>
       </c>
       <c r="F90" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3643,7 +3628,7 @@
         <v>241</v>
       </c>
       <c r="F91" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3663,7 +3648,7 @@
         <v>241</v>
       </c>
       <c r="F92" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3683,7 +3668,7 @@
         <v>241</v>
       </c>
       <c r="F93" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3703,7 +3688,7 @@
         <v>241</v>
       </c>
       <c r="F94" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3723,7 +3708,7 @@
         <v>241</v>
       </c>
       <c r="F95" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3743,7 +3728,7 @@
         <v>241</v>
       </c>
       <c r="F96" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3763,7 +3748,7 @@
         <v>241</v>
       </c>
       <c r="F97" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3783,7 +3768,7 @@
         <v>241</v>
       </c>
       <c r="F98" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3803,7 +3788,7 @@
         <v>241</v>
       </c>
       <c r="F99" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3823,7 +3808,7 @@
         <v>241</v>
       </c>
       <c r="F100" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3843,7 +3828,7 @@
         <v>241</v>
       </c>
       <c r="F101" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3863,7 +3848,7 @@
         <v>241</v>
       </c>
       <c r="F102" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3883,7 +3868,7 @@
         <v>241</v>
       </c>
       <c r="F103" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3903,7 +3888,7 @@
         <v>241</v>
       </c>
       <c r="F104" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3923,7 +3908,7 @@
         <v>242</v>
       </c>
       <c r="F105" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3943,7 +3928,7 @@
         <v>242</v>
       </c>
       <c r="F106" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3963,7 +3948,7 @@
         <v>242</v>
       </c>
       <c r="F107" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3983,7 +3968,7 @@
         <v>242</v>
       </c>
       <c r="F108" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -4003,7 +3988,7 @@
         <v>242</v>
       </c>
       <c r="F109" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -4023,7 +4008,7 @@
         <v>242</v>
       </c>
       <c r="F110" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -4043,7 +4028,7 @@
         <v>242</v>
       </c>
       <c r="F111" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -4063,7 +4048,7 @@
         <v>242</v>
       </c>
       <c r="F112" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4083,11 +4068,9 @@
         <v>242</v>
       </c>
       <c r="F113" t="s">
-        <v>367</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>370</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="G113" s="3"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
@@ -4106,11 +4089,9 @@
         <v>242</v>
       </c>
       <c r="F114" t="s">
-        <v>368</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>369</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="G114" s="3"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -4129,7 +4110,7 @@
         <v>242</v>
       </c>
       <c r="F115" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4149,7 +4130,7 @@
         <v>242</v>
       </c>
       <c r="F116" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4169,7 +4150,7 @@
         <v>242</v>
       </c>
       <c r="F117" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4189,11 +4170,9 @@
         <v>242</v>
       </c>
       <c r="F118" t="s">
-        <v>374</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>375</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="I118" s="3"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -4212,31 +4191,20 @@
         <v>242</v>
       </c>
       <c r="F119" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E120" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F121" s="3"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
         <v>262</v>
       </c>
-      <c r="F120" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F121" t="s">
-        <v>264</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F120" r:id="rId1"/>
-    <hyperlink ref="G114" r:id="rId2"/>
-    <hyperlink ref="G113" r:id="rId3"/>
-    <hyperlink ref="I118" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>